<commit_message>
Additional subsampling and metrics testing
</commit_message>
<xml_diff>
--- a/data/compile_2015-2019/field_data/2015_LGSS_data_MASTER_oct2020_siteIDcorrections.xlsx
+++ b/data/compile_2015-2019/field_data/2015_LGSS_data_MASTER_oct2020_siteIDcorrections.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\LGSS_scripting\lgss\data\compile_2015-2019\field_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E172D3F-3A4F-47E5-B515-BD887985A0F2}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9C10127-C7B9-499A-8EFA-D978EE75EF72}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2520" yWindow="405" windowWidth="19200" windowHeight="13245" tabRatio="638" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="10690" windowWidth="19420" windowHeight="11020" tabRatio="638" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FieldData" sheetId="3" r:id="rId1"/>
@@ -31,7 +31,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -149,7 +151,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3378" uniqueCount="1234">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3377" uniqueCount="1233">
   <si>
     <t>Direct</t>
   </si>
@@ -3680,9 +3682,6 @@
   </si>
   <si>
     <t>LU rounds up to 75. Add as ref site?</t>
-  </si>
-  <si>
-    <t>LU rounds up to 75. Add as ref site? But 424 cond…</t>
   </si>
   <si>
     <t>Non-ref site? Habitat scores are low, notes "Stream is surrounded on all sides by agricultural fields". Much of basin is high natural LU, but site is very ag heavy. Note says lots of dumping at site.</t>
@@ -4870,9 +4869,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:BC97"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" topLeftCell="AK1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A75" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AA83" sqref="A83:XFD83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4979,7 +4978,7 @@
         <v>9</v>
       </c>
       <c r="S1" s="7" t="s">
-        <v>1199</v>
+        <v>1198</v>
       </c>
       <c r="T1" s="7" t="s">
         <v>10</v>
@@ -5036,22 +5035,22 @@
         <v>28</v>
       </c>
       <c r="AL1" s="19" t="s">
-        <v>1198</v>
+        <v>1197</v>
       </c>
       <c r="AM1" s="7" t="s">
         <v>854</v>
       </c>
       <c r="AN1" s="19" t="s">
+        <v>1182</v>
+      </c>
+      <c r="AO1" s="19" t="s">
         <v>1183</v>
       </c>
-      <c r="AO1" s="19" t="s">
-        <v>1184</v>
-      </c>
       <c r="AP1" s="6" t="s">
-        <v>1180</v>
+        <v>1179</v>
       </c>
       <c r="AQ1" s="19" t="s">
-        <v>1228</v>
+        <v>1227</v>
       </c>
       <c r="AR1" s="19"/>
       <c r="AS1" s="19"/>
@@ -5105,7 +5104,7 @@
         <v>294</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>1232</v>
+        <v>1231</v>
       </c>
       <c r="O2" s="2" t="s">
         <v>295</v>
@@ -5546,7 +5545,7 @@
     </row>
     <row r="6" spans="1:55" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>1229</v>
+        <v>1228</v>
       </c>
       <c r="B6" s="19" t="s">
         <v>953</v>
@@ -5645,7 +5644,7 @@
         <v>64.992405590000004</v>
       </c>
       <c r="AM6" s="2" t="s">
-        <v>1229</v>
+        <v>1228</v>
       </c>
       <c r="AN6" s="19" t="s">
         <v>949</v>
@@ -6988,7 +6987,7 @@
     </row>
     <row r="17" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>1230</v>
+        <v>1229</v>
       </c>
       <c r="B17" s="19" t="s">
         <v>964</v>
@@ -7100,7 +7099,7 @@
         <v>39.115418890000001</v>
       </c>
       <c r="AM17" s="2" t="s">
-        <v>1230</v>
+        <v>1229</v>
       </c>
       <c r="AN17" s="19" t="s">
         <v>949</v>
@@ -8733,7 +8732,7 @@
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
       <c r="F30" s="2" t="s">
-        <v>1227</v>
+        <v>1226</v>
       </c>
       <c r="G30" s="19">
         <v>42.289520000000003</v>
@@ -8980,7 +8979,7 @@
         <v>0</v>
       </c>
       <c r="AQ31" s="2" t="s">
-        <v>1182</v>
+        <v>1181</v>
       </c>
       <c r="AR31" s="19"/>
       <c r="AS31" s="19"/>
@@ -11939,7 +11938,7 @@
         <v>0</v>
       </c>
       <c r="AQ53" s="2" t="s">
-        <v>1178</v>
+        <v>1177</v>
       </c>
       <c r="AR53" s="19"/>
       <c r="AS53" s="19"/>
@@ -12216,7 +12215,7 @@
         <v>1</v>
       </c>
       <c r="AQ55" s="2" t="s">
-        <v>1181</v>
+        <v>1180</v>
       </c>
       <c r="AR55" s="19"/>
       <c r="AS55" s="19"/>
@@ -13735,7 +13734,7 @@
       <c r="D67" s="2"/>
       <c r="E67" s="2"/>
       <c r="F67" s="2" t="s">
-        <v>1226</v>
+        <v>1225</v>
       </c>
       <c r="G67" s="19">
         <v>43.078451999999899</v>
@@ -14125,7 +14124,7 @@
     </row>
     <row r="70" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A70" s="15" t="s">
-        <v>1231</v>
+        <v>1230</v>
       </c>
       <c r="B70" s="19" t="s">
         <v>1018</v>
@@ -14229,7 +14228,7 @@
         <v>99.298801179999998</v>
       </c>
       <c r="AM70" s="15" t="s">
-        <v>1231</v>
+        <v>1230</v>
       </c>
       <c r="AN70" s="19" t="s">
         <v>969</v>
@@ -15744,7 +15743,7 @@
         <v>937</v>
       </c>
       <c r="B82" s="19" t="s">
-        <v>1030</v>
+        <v>1031</v>
       </c>
       <c r="C82" s="23">
         <v>16</v>
@@ -15843,8 +15842,8 @@
         <v>0.04</v>
       </c>
       <c r="AK82" s="2"/>
-      <c r="AL82" s="31">
-        <v>74.554904350000001</v>
+      <c r="AL82" s="19">
+        <v>57.666355240000001</v>
       </c>
       <c r="AM82" s="2" t="s">
         <v>937</v>
@@ -15853,16 +15852,14 @@
         <v>949</v>
       </c>
       <c r="AO82" s="19" t="str">
-        <f t="shared" si="4"/>
-        <v>ref</v>
+        <f>IF(AL82&gt;=74.5,"ref","test")</f>
+        <v>test</v>
       </c>
       <c r="AP82" s="1">
-        <f t="shared" si="5"/>
+        <f>IF(AH83&lt;250,1,0)</f>
         <v>0</v>
       </c>
-      <c r="AQ82" s="2" t="s">
-        <v>1177</v>
-      </c>
+      <c r="AQ82" s="2"/>
       <c r="AR82" s="19"/>
       <c r="AS82" s="19"/>
       <c r="AT82" s="19"/>
@@ -15881,7 +15878,7 @@
         <v>910</v>
       </c>
       <c r="B83" s="19" t="s">
-        <v>1031</v>
+        <v>1030</v>
       </c>
       <c r="C83" s="23">
         <v>16</v>
@@ -15980,8 +15977,8 @@
         <v>0.74</v>
       </c>
       <c r="AK83" s="2"/>
-      <c r="AL83" s="19">
-        <v>57.666355240000001</v>
+      <c r="AL83" s="31">
+        <v>74.554904350000001</v>
       </c>
       <c r="AM83" s="20" t="s">
         <v>910</v>
@@ -15990,11 +15987,11 @@
         <v>949</v>
       </c>
       <c r="AO83" s="19" t="str">
-        <f t="shared" si="4"/>
-        <v>test</v>
+        <f>IF(AL83&gt;=74.5,"ref","test")</f>
+        <v>ref</v>
       </c>
       <c r="AP83" s="1">
-        <f t="shared" si="5"/>
+        <f>IF(AH82&lt;250,1,0)</f>
         <v>0</v>
       </c>
       <c r="AQ83" s="19"/>
@@ -16123,7 +16120,7 @@
         <v>0</v>
       </c>
       <c r="AQ84" s="2" t="s">
-        <v>1179</v>
+        <v>1178</v>
       </c>
       <c r="AR84" s="19"/>
       <c r="AS84" s="19"/>
@@ -17834,13 +17831,9 @@
       <c r="BC97" s="19"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AQ97" xr:uid="{25EE624E-A8EC-44DE-B895-50CDBBABAEB7}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:AQ97">
-      <sortCondition ref="A8"/>
-    </sortState>
-  </autoFilter>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:AQ97">
-    <sortCondition descending="1" ref="AL8"/>
+  <autoFilter ref="A1:AQ97" xr:uid="{25EE624E-A8EC-44DE-B895-50CDBBABAEB7}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B83">
+    <sortCondition ref="B82"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -19577,7 +19570,7 @@
     </row>
     <row r="6" spans="1:461" x14ac:dyDescent="0.25">
       <c r="A6" s="17" t="s">
-        <v>1229</v>
+        <v>1228</v>
       </c>
       <c r="E6" s="17">
         <v>1</v>
@@ -20613,7 +20606,7 @@
     </row>
     <row r="17" spans="1:461" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>1230</v>
+        <v>1229</v>
       </c>
       <c r="K17" s="17">
         <v>2</v>
@@ -26053,7 +26046,7 @@
     </row>
     <row r="70" spans="1:461" x14ac:dyDescent="0.25">
       <c r="A70" s="17" t="s">
-        <v>1231</v>
+        <v>1230</v>
       </c>
       <c r="B70" s="17">
         <v>2</v>
@@ -29013,43 +29006,43 @@
         <v>385</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>1197</v>
+        <v>1196</v>
       </c>
       <c r="D1" s="8" t="s">
+        <v>1184</v>
+      </c>
+      <c r="E1" s="8" t="s">
         <v>1185</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="F1" s="8" t="s">
         <v>1186</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="G1" s="8" t="s">
         <v>1187</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="H1" s="8" t="s">
         <v>1188</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="I1" s="8" t="s">
+        <v>1195</v>
+      </c>
+      <c r="J1" s="8" t="s">
         <v>1189</v>
       </c>
-      <c r="I1" s="8" t="s">
-        <v>1196</v>
-      </c>
-      <c r="J1" s="8" t="s">
+      <c r="K1" s="8" t="s">
         <v>1190</v>
       </c>
-      <c r="K1" s="8" t="s">
+      <c r="L1" s="8" t="s">
         <v>1191</v>
       </c>
-      <c r="L1" s="8" t="s">
+      <c r="M1" s="8" t="s">
         <v>1192</v>
       </c>
-      <c r="M1" s="8" t="s">
+      <c r="N1" s="8" t="s">
         <v>1193</v>
       </c>
-      <c r="N1" s="8" t="s">
+      <c r="O1" s="8" t="s">
         <v>1194</v>
-      </c>
-      <c r="O1" s="8" t="s">
-        <v>1195</v>
       </c>
       <c r="P1" s="8" t="s">
         <v>360</v>
@@ -29102,7 +29095,7 @@
         <v>8</v>
       </c>
       <c r="P2" s="4" t="s">
-        <v>1233</v>
+        <v>1232</v>
       </c>
     </row>
     <row r="3" spans="1:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
@@ -29255,7 +29248,7 @@
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>1229</v>
+        <v>1228</v>
       </c>
       <c r="B6" s="3">
         <v>42221</v>
@@ -29793,7 +29786,7 @@
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>1230</v>
+        <v>1229</v>
       </c>
       <c r="B17" s="3">
         <v>42206</v>
@@ -32311,7 +32304,7 @@
     </row>
     <row r="69" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A69" s="4" t="s">
-        <v>1231</v>
+        <v>1230</v>
       </c>
       <c r="B69" s="3">
         <v>42174</v>
@@ -33721,7 +33714,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>1229</v>
+        <v>1228</v>
       </c>
       <c r="B5" s="10">
         <v>4.191616766467007</v>
@@ -33785,7 +33778,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>1230</v>
+        <v>1229</v>
       </c>
       <c r="B13" s="10">
         <v>3.5842293906809886</v>
@@ -34129,7 +34122,7 @@
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
-        <v>1231</v>
+        <v>1230</v>
       </c>
       <c r="B56" s="10">
         <v>2.173913043478251</v>
@@ -34387,7 +34380,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>1229</v>
+        <v>1228</v>
       </c>
       <c r="B3" s="11">
         <v>1.4041916167664672</v>
@@ -34450,7 +34443,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>1230</v>
+        <v>1229</v>
       </c>
       <c r="B10" s="11">
         <v>1.5999999999999999</v>
@@ -34774,7 +34767,7 @@
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
-        <v>1231</v>
+        <v>1230</v>
       </c>
       <c r="B46" s="11">
         <v>1.3895253682487723</v>
@@ -35267,7 +35260,7 @@
     </row>
     <row r="6" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>1229</v>
+        <v>1228</v>
       </c>
       <c r="B6" s="19">
         <v>83</v>
@@ -35751,7 +35744,7 @@
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>1230</v>
+        <v>1229</v>
       </c>
       <c r="B17" s="19">
         <v>83</v>
@@ -38083,7 +38076,7 @@
     </row>
     <row r="70" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A70" s="15" t="s">
-        <v>1231</v>
+        <v>1230</v>
       </c>
       <c r="B70" s="19">
         <v>58</v>
@@ -39341,82 +39334,82 @@
         <v>1</v>
       </c>
       <c r="B1" s="35" t="s">
+        <v>1199</v>
+      </c>
+      <c r="C1" s="35" t="s">
         <v>1200</v>
       </c>
-      <c r="C1" s="35" t="s">
+      <c r="D1" s="35" t="s">
         <v>1201</v>
       </c>
-      <c r="D1" s="35" t="s">
+      <c r="E1" s="35" t="s">
         <v>1202</v>
       </c>
-      <c r="E1" s="35" t="s">
+      <c r="F1" s="35" t="s">
         <v>1203</v>
       </c>
-      <c r="F1" s="35" t="s">
+      <c r="G1" s="35" t="s">
         <v>1204</v>
       </c>
-      <c r="G1" s="35" t="s">
+      <c r="H1" s="35" t="s">
         <v>1205</v>
       </c>
-      <c r="H1" s="35" t="s">
+      <c r="I1" s="35" t="s">
         <v>1206</v>
       </c>
-      <c r="I1" s="35" t="s">
+      <c r="J1" s="35" t="s">
         <v>1207</v>
       </c>
-      <c r="J1" s="35" t="s">
+      <c r="K1" s="35" t="s">
         <v>1208</v>
       </c>
-      <c r="K1" s="35" t="s">
+      <c r="L1" s="35" t="s">
         <v>1209</v>
       </c>
-      <c r="L1" s="35" t="s">
+      <c r="M1" s="35" t="s">
         <v>1210</v>
       </c>
-      <c r="M1" s="35" t="s">
+      <c r="N1" s="35" t="s">
         <v>1211</v>
       </c>
-      <c r="N1" s="35" t="s">
+      <c r="O1" s="35" t="s">
         <v>1212</v>
       </c>
-      <c r="O1" s="35" t="s">
+      <c r="P1" s="35" t="s">
         <v>1213</v>
       </c>
-      <c r="P1" s="35" t="s">
+      <c r="Q1" s="35" t="s">
         <v>1214</v>
       </c>
-      <c r="Q1" s="35" t="s">
+      <c r="R1" s="35" t="s">
         <v>1215</v>
       </c>
-      <c r="R1" s="35" t="s">
+      <c r="S1" s="35" t="s">
         <v>1216</v>
       </c>
-      <c r="S1" s="35" t="s">
+      <c r="T1" s="35" t="s">
         <v>1217</v>
       </c>
-      <c r="T1" s="35" t="s">
+      <c r="U1" s="36" t="s">
         <v>1218</v>
       </c>
-      <c r="U1" s="36" t="s">
+      <c r="V1" s="35" t="s">
         <v>1219</v>
       </c>
-      <c r="V1" s="35" t="s">
+      <c r="W1" s="35" t="s">
         <v>1220</v>
       </c>
-      <c r="W1" s="35" t="s">
+      <c r="X1" s="35" t="s">
         <v>1221</v>
       </c>
-      <c r="X1" s="35" t="s">
+      <c r="Y1" s="35" t="s">
         <v>1222</v>
       </c>
-      <c r="Y1" s="35" t="s">
+      <c r="Z1" s="35" t="s">
         <v>1223</v>
       </c>
-      <c r="Z1" s="35" t="s">
+      <c r="AA1" s="36" t="s">
         <v>1224</v>
-      </c>
-      <c r="AA1" s="36" t="s">
-        <v>1225</v>
       </c>
     </row>
     <row r="2" spans="1:27" x14ac:dyDescent="0.25">
@@ -39753,7 +39746,7 @@
     </row>
     <row r="6" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A6" s="19" t="s">
-        <v>1229</v>
+        <v>1228</v>
       </c>
       <c r="B6" s="19">
         <v>4120103</v>
@@ -40666,7 +40659,7 @@
     </row>
     <row r="17" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A17" s="19" t="s">
-        <v>1230</v>
+        <v>1229</v>
       </c>
       <c r="B17" s="19">
         <v>4150102</v>
@@ -45065,7 +45058,7 @@
     </row>
     <row r="70" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A70" s="19" t="s">
-        <v>1231</v>
+        <v>1230</v>
       </c>
       <c r="B70" s="19">
         <v>2020002</v>

</xml_diff>